<commit_message>
nowe kryt dla cial skonczonych
</commit_message>
<xml_diff>
--- a/Wyniki.xlsx
+++ b/Wyniki.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szymon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szymon\Desktop\IntersectionsOfStraightLines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D4062-F5A7-4EC7-875F-9D94BEF13AAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A246E48-0CC2-4498-8518-6D14471C93DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="330" windowWidth="21600" windowHeight="10545" xr2:uid="{F58720EC-6F02-4227-9518-32D818808B2C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F58720EC-6F02-4227-9518-32D818808B2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="18">
   <si>
     <t>d</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>do oczekiwanego czasu dane (bez naprawionego minimum)</t>
+  </si>
+  <si>
+    <t>&lt;-3,95 dnia</t>
   </si>
 </sst>
 </file>
@@ -566,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0968E3D0-9704-4F78-891B-E294D0D7D6D7}">
   <dimension ref="D1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +714,7 @@
         <v>0.47399999999999998</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U13" si="5">IF(T3=0,0,T4/T3)</f>
+        <f t="shared" ref="U3:U11" si="5">IF(T3=0,0,T4/T3)</f>
         <v>1.5632911392405064</v>
       </c>
     </row>
@@ -747,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M3:M40" si="6">IF(L3=0,0,L4/L3)</f>
+        <f t="shared" ref="M4:M40" si="6">IF(L3=0,0,L4/L3)</f>
         <v>0</v>
       </c>
       <c r="N4" s="3">
@@ -2593,11 +2596,10 @@
         <v>11</v>
       </c>
       <c r="P40" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>341301</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>